<commit_message>
Added area, volume, density, temperature conversions
</commit_message>
<xml_diff>
--- a/kb/unit-converter/length.xlsx
+++ b/kb/unit-converter/length.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Measure Label</t>
   </si>
@@ -28,13 +28,22 @@
     <t xml:space="preserve">Length</t>
   </si>
   <si>
+    <t xml:space="preserve">Cell B2 Must be the name of the measure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Decimal Places</t>
   </si>
   <si>
+    <t xml:space="preserve">Cell B3 must be an integer, it controls number of decimal places used in the converter output for this measure.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Image</t>
   </si>
   <si>
     <t xml:space="preserve">length.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icon, must be populated.  The png should be in the images directory of the edb source folder</t>
   </si>
   <si>
     <t xml:space="preserve">Units</t>
@@ -55,7 +64,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">&lt; The first unit of measure should </t>
+      <t xml:space="preserve">The first unit of measure should </t>
     </r>
     <r>
       <rPr>
@@ -79,7 +88,13 @@
     <t xml:space="preserve">Millimeters</t>
   </si>
   <si>
+    <t xml:space="preserve">For all other units, the factor should be the DIVISOR, in order to get from the unit on this row, to the standard unit in row 6.  For example, if you have 5000mm, then dividing by 1000 gets you 5 meters.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can place as many units as you want – the system will read until there is an empty cell in column A</t>
   </si>
   <si>
     <t xml:space="preserve">Inches</t>
@@ -92,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -112,6 +127,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -120,12 +141,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,9 +189,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -176,6 +223,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -187,87 +294,107 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="46.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="C7" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>3.28083989501312</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>39.3701</v>
       </c>
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
kb changes for friction losses
</commit_message>
<xml_diff>
--- a/kb/unit-converter/length.xlsx
+++ b/kb/unit-converter/length.xlsx
@@ -63,6 +63,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">The first unit of measure should </t>
     </r>
@@ -72,6 +73,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">always</t>
     </r>
@@ -80,6 +82,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> have a factor of 1.  All other factors relate to this default unit. You may choose any unit for this, and the system will perform all conversions between any listed unit of measure.</t>
     </r>
@@ -112,6 +115,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,12 +137,14 @@
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -294,7 +300,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Last mods before beta
</commit_message>
<xml_diff>
--- a/kb/unit-converter/length.xlsx
+++ b/kb/unit-converter/length.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_0F194150FFF509CEFE033E1A28E931EB91749AE1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A029CA63-13CD-4D3A-B02D-7DE0FDBDFF5F}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\edb\kb\unit-converter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720C20D5-D615-4A07-ADFD-5272B4A76376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1500" windowWidth="12465" windowHeight="11280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -598,10 +603,10 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A6" sqref="A6:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
@@ -609,7 +614,7 @@
     <col min="4" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -631,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -642,14 +647,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.149999999999999">
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -658,7 +663,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="54.75" customHeight="1">
+    <row r="6" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -669,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="46.5">
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -680,43 +685,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="24">
+    <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="1">
-        <v>3.280833436679587</v>
+        <v>3.2808398950000002</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1">
-        <v>39.370078740157481</v>
+        <v>39.370078739999997</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10">
-        <v>6.2137119223733392E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>6.2137100000000001E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11">
-        <v>1.0936132983377078</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>1.093613298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -724,23 +729,23 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
       <c r="B13">
-        <v>39370.078740157478</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>39370.078739999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
       <c r="B14">
-        <v>39370078.740157485</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>39370078.740000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -748,7 +753,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -756,20 +761,20 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17">
-        <v>6.2137003393301752E-4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>6.2137E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
       <c r="B18">
-        <v>3.280833436679587</v>
+        <v>3.2808334370000001</v>
       </c>
     </row>
   </sheetData>
@@ -783,6 +788,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8da57d07-bd53-4918-9441-156ccef8128a">
@@ -791,15 +805,6 @@
     <TaxCatchAll xmlns="32f445ef-0db1-4ff5-a403-59aa008b5549" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,13 +1045,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6921C4C-98D7-422D-A8FE-A6F7F50B9F48}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A67F428-3A37-4E5C-BCB7-816FA14B903C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A67F428-3A37-4E5C-BCB7-816FA14B903C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6921C4C-98D7-422D-A8FE-A6F7F50B9F48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8da57d07-bd53-4918-9441-156ccef8128a"/>
+    <ds:schemaRef ds:uri="32f445ef-0db1-4ff5-a403-59aa008b5549"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5DE202-A740-4713-A379-5C0AA5AC1B2C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5DE202-A740-4713-A379-5C0AA5AC1B2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8da57d07-bd53-4918-9441-156ccef8128a"/>
+    <ds:schemaRef ds:uri="32f445ef-0db1-4ff5-a403-59aa008b5549"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>